<commit_message>
hoàn thành phần tạo pan 27.12.2023
</commit_message>
<xml_diff>
--- a/Đo_An/HoanThanhDangNhap/bin/Debug/Resources/Du lieu cau hoi/thu vien comp.xlsx
+++ b/Đo_An/HoanThanhDangNhap/bin/Debug/Resources/Du lieu cau hoi/thu vien comp.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26501"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27029"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\lam do an\Qua trinh CODE C#\DangHoanThien2504\student_add bai hoc_ 0904\student_add bai hoc\HoanThanhDangNhap\bin\Debug\Resources\Du lieu cau hoi\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Đăng_Quý_UTE_K19\Đo_An\HoanThanhDangNhap\bin\Debug\Resources\Du lieu cau hoi\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{32E601A6-5964-4CF3-B82E-9C3998663D29}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BC1F15AB-7C96-4839-B58D-FB88AAAFEA48}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{44CE0958-A6C1-42E6-8D55-7FA2B2385169}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{44CE0958-A6C1-42E6-8D55-7FA2B2385169}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="130" uniqueCount="78">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="212" uniqueCount="85">
   <si>
     <t>3</t>
   </si>
@@ -82,93 +82,12 @@
     <t>\\Resources\\tong hop final wiring\\c7.png</t>
   </si>
   <si>
-    <t>\\Resources\\tong hop final wiring\\c8.png</t>
-  </si>
-  <si>
-    <t>Relay còi (#9)</t>
-  </si>
-  <si>
-    <t>Còi (#11)</t>
-  </si>
-  <si>
-    <t>Công tắc còi (#17)</t>
-  </si>
-  <si>
-    <t>GND</t>
-  </si>
-  <si>
-    <t>Công tắc đèn lùi (#10)</t>
-  </si>
-  <si>
     <t>comp8</t>
   </si>
   <si>
-    <t>Công tắc đèn phanh (#2)</t>
-  </si>
-  <si>
-    <t>Công tắc đèn đầu (#8)</t>
-  </si>
-  <si>
-    <t>Đèn phanh trái (#12)</t>
-  </si>
-  <si>
-    <t>Đèn đuôi trái (#13)</t>
-  </si>
-  <si>
-    <t>Công tắc P/N (#8)</t>
-  </si>
-  <si>
-    <t>Relay máy đề (#9)</t>
-  </si>
-  <si>
-    <t>Công tắc đánh lửa (#10)</t>
-  </si>
-  <si>
-    <t>Motor máy đề (#16)</t>
-  </si>
-  <si>
-    <t>Bộ chớp (flasher) (#2)</t>
-  </si>
-  <si>
-    <t>Công tắc đèn báo đỗ (#10)</t>
-  </si>
-  <si>
-    <t>Đèn báo bên hông (#13)</t>
-  </si>
-  <si>
     <t>comp9</t>
   </si>
   <si>
-    <t>Điện trở #3</t>
-  </si>
-  <si>
-    <t>Điện trở #7</t>
-  </si>
-  <si>
-    <t>Công tắc đèn (#8)</t>
-  </si>
-  <si>
-    <t>Công tắc đèn mờ (#10)</t>
-  </si>
-  <si>
-    <t>Đèn pha trái (#12)</t>
-  </si>
-  <si>
-    <t>Đèn cốt trái (#13)</t>
-  </si>
-  <si>
-    <t>Đèn #12</t>
-  </si>
-  <si>
-    <t>Đèn #15</t>
-  </si>
-  <si>
-    <t>Công tắc xinhan (#8)</t>
-  </si>
-  <si>
-    <t>Đèn xinhan (#15)</t>
-  </si>
-  <si>
     <t>1</t>
   </si>
   <si>
@@ -181,39 +100,9 @@
     <t>\\Resources\\tong hop final wiring\\c1.png</t>
   </si>
   <si>
-    <t>\\Resources\\tong hop final wiring\\c2.png</t>
-  </si>
-  <si>
     <t>\\Resources\\tong hop final wiring\\c3.png</t>
   </si>
   <si>
-    <t>Điện trở #4</t>
-  </si>
-  <si>
-    <t>Điện trở #5</t>
-  </si>
-  <si>
-    <t>Đèn đuôi phải (#14)</t>
-  </si>
-  <si>
-    <t>Đèn phanh phải (#15)</t>
-  </si>
-  <si>
-    <t>Đèn đỗ (#12)</t>
-  </si>
-  <si>
-    <t>Đèn báo rẽ (#14)</t>
-  </si>
-  <si>
-    <t>Đèn cốt phải (#14)</t>
-  </si>
-  <si>
-    <t>Đèn pha phải (#15)</t>
-  </si>
-  <si>
-    <t>Cầu chì ngắt mạch (#1)</t>
-  </si>
-  <si>
     <t>Chương 1</t>
   </si>
   <si>
@@ -260,13 +149,145 @@
   </si>
   <si>
     <t xml:space="preserve"> Cầu chì ngắt mạch (#1), Công tắc đèn (#8), Công tắc đèn mờ (#10), Đèn pha trái (#12), Đèn cốt trái (#13), Đèn cốt phải (#14), Đèn pha phải (#15), GND</t>
+  </si>
+  <si>
+    <t>9</t>
+  </si>
+  <si>
+    <t>11</t>
+  </si>
+  <si>
+    <t>12</t>
+  </si>
+  <si>
+    <t>13</t>
+  </si>
+  <si>
+    <t>14</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Đường dây E2 </t>
+  </si>
+  <si>
+    <t>đường dây +B</t>
+  </si>
+  <si>
+    <t>Đường Dây VG</t>
+  </si>
+  <si>
+    <t>Đường dây THA</t>
+  </si>
+  <si>
+    <t>Đường dây EVG</t>
+  </si>
+  <si>
+    <t>10</t>
+  </si>
+  <si>
+    <t>Đường Dây KS</t>
+  </si>
+  <si>
+    <t>Đường dây PA</t>
+  </si>
+  <si>
+    <t>Đường dây E2</t>
+  </si>
+  <si>
+    <t>đường dây VC</t>
+  </si>
+  <si>
+    <t>Đường Dây VS</t>
+  </si>
+  <si>
+    <t>Đường dây FC</t>
+  </si>
+  <si>
+    <t>Đường Dây PIM</t>
+  </si>
+  <si>
+    <t>Đường Dây NE+</t>
+  </si>
+  <si>
+    <t>đường dây TH</t>
+  </si>
+  <si>
+    <t>đường dây PSW</t>
+  </si>
+  <si>
+    <t>Đường Dây IDL</t>
+  </si>
+  <si>
+    <t>đường dây VTA</t>
+  </si>
+  <si>
+    <t>Đường Dây VC</t>
+  </si>
+  <si>
+    <t>Đường Dây STA</t>
+  </si>
+  <si>
+    <t>Đường Dây IG</t>
+  </si>
+  <si>
+    <t>Đường Dây GND</t>
+  </si>
+  <si>
+    <t>5</t>
+  </si>
+  <si>
+    <t>đường dây FP</t>
+  </si>
+  <si>
+    <t>Đường Dây +B</t>
+  </si>
+  <si>
+    <t>Đường dây +B</t>
+  </si>
+  <si>
+    <t>đường dây IGT</t>
+  </si>
+  <si>
+    <t>đường dây #10</t>
+  </si>
+  <si>
+    <t>Đường dây VC hoặc VCPA,VCPA2</t>
+  </si>
+  <si>
+    <t>đường dây E2 hoặc EPA,EPA2</t>
+  </si>
+  <si>
+    <t>Đường Dây VPA</t>
+  </si>
+  <si>
+    <t>Đường Dây VPA2</t>
+  </si>
+  <si>
+    <t>Đường Dây VPA và VPA2</t>
+  </si>
+  <si>
+    <t>Đường Dây VTA</t>
+  </si>
+  <si>
+    <t>Đường Dây VTA2</t>
+  </si>
+  <si>
+    <t>Đường Dây VTA và VTA2</t>
+  </si>
+  <si>
+    <t>comp10</t>
+  </si>
+  <si>
+    <t>Đường Dây M+</t>
+  </si>
+  <si>
+    <t>Đường Dây M-</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -282,6 +303,26 @@
     </font>
     <font>
       <u/>
+      <sz val="11"/>
+      <color theme="10"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="8"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <sz val="11"/>
       <color theme="10"/>
       <name val="Calibri"/>
@@ -331,14 +372,20 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="49" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="49" fontId="1" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="49" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="49" fontId="2" fillId="0" borderId="1" xfId="1" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="49" fontId="2" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="49" fontId="2" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="5" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -654,19 +701,21 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{45D2A3BD-74E5-49D8-B5E0-F6FA57BFF832}">
-  <dimension ref="A1:K17"/>
+  <dimension ref="A1:L29"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G3" sqref="G3"/>
+    <sheetView tabSelected="1" topLeftCell="F1" workbookViewId="0">
+      <selection activeCell="M19" sqref="M19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="24.77734375" defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="14.33203125" style="1" customWidth="1"/>
-    <col min="2" max="16384" width="24.77734375" style="1"/>
+    <col min="2" max="10" width="24.77734375" style="1"/>
+    <col min="11" max="11" width="13.5546875" style="1" bestFit="1" customWidth="1"/>
+    <col min="12" max="16384" width="24.77734375" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
         <v>11</v>
       </c>
@@ -692,103 +741,112 @@
         <v>4</v>
       </c>
       <c r="I1" s="2" t="s">
-        <v>24</v>
+        <v>18</v>
       </c>
       <c r="J1" s="2" t="s">
-        <v>36</v>
+        <v>19</v>
       </c>
       <c r="K1" s="2" t="s">
+        <v>82</v>
+      </c>
+      <c r="L1" s="2" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:11" ht="14.4" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:12" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A2" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="B2" s="3" t="s">
+        <v>46</v>
+      </c>
+      <c r="C2" s="3" t="s">
         <v>47</v>
       </c>
-      <c r="B2" s="3" t="s">
-        <v>61</v>
-      </c>
-      <c r="C2" s="3" t="s">
-        <v>37</v>
-      </c>
       <c r="D2" s="3" t="s">
+        <v>48</v>
+      </c>
+      <c r="E2" s="3" t="s">
+        <v>49</v>
+      </c>
+      <c r="F2" s="3" t="s">
+        <v>50</v>
+      </c>
+      <c r="G2" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="H2" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="I2" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="J2" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="K2" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="L2" s="4" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="3" spans="1:12" ht="14.4" x14ac:dyDescent="0.3">
+      <c r="A3" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="B3" s="3" t="s">
+        <v>54</v>
+      </c>
+      <c r="C3" s="3" t="s">
+        <v>47</v>
+      </c>
+      <c r="D3" s="3" t="s">
+        <v>52</v>
+      </c>
+      <c r="E3" s="3" t="s">
+        <v>49</v>
+      </c>
+      <c r="F3" s="3" t="s">
         <v>53</v>
       </c>
-      <c r="E2" s="3" t="s">
-        <v>38</v>
-      </c>
-      <c r="F2" s="3" t="s">
-        <v>22</v>
-      </c>
-      <c r="G2" s="3" t="s">
-        <v>1</v>
-      </c>
-      <c r="H2" s="3" t="s">
-        <v>1</v>
-      </c>
-      <c r="I2" s="3" t="s">
-        <v>1</v>
-      </c>
-      <c r="J2" s="3" t="s">
-        <v>1</v>
-      </c>
-      <c r="K2" s="4" t="s">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="3" spans="1:11" ht="14.4" x14ac:dyDescent="0.3">
-      <c r="A3" s="3" t="s">
-        <v>48</v>
-      </c>
-      <c r="B3" s="3" t="s">
-        <v>61</v>
-      </c>
-      <c r="C3" s="3" t="s">
-        <v>37</v>
-      </c>
-      <c r="D3" s="3" t="s">
-        <v>53</v>
-      </c>
-      <c r="E3" s="3" t="s">
-        <v>54</v>
-      </c>
-      <c r="F3" s="3" t="s">
-        <v>38</v>
-      </c>
-      <c r="G3" s="3" t="s">
-        <v>22</v>
-      </c>
-      <c r="H3" s="3" t="s">
-        <v>1</v>
-      </c>
-      <c r="I3" s="3" t="s">
-        <v>1</v>
-      </c>
-      <c r="J3" s="3" t="s">
-        <v>1</v>
-      </c>
-      <c r="K3" s="4" t="s">
-        <v>51</v>
-      </c>
-    </row>
-    <row r="4" spans="1:11" ht="14.4" x14ac:dyDescent="0.3">
+      <c r="G3" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="H3" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="I3" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="J3" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="K3" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="L3" s="4" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="4" spans="1:12" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A4" s="3" t="s">
         <v>0</v>
       </c>
       <c r="B4" s="3" t="s">
-        <v>61</v>
+        <v>46</v>
       </c>
       <c r="C4" s="3" t="s">
-        <v>19</v>
+        <v>55</v>
       </c>
       <c r="D4" s="3" t="s">
-        <v>20</v>
+        <v>56</v>
       </c>
       <c r="E4" s="3" t="s">
-        <v>21</v>
+        <v>49</v>
       </c>
       <c r="F4" s="3" t="s">
-        <v>22</v>
+        <v>57</v>
       </c>
       <c r="G4" s="3" t="s">
         <v>1</v>
@@ -802,101 +860,110 @@
       <c r="J4" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="K4" s="4" t="s">
-        <v>52</v>
-      </c>
-    </row>
-    <row r="5" spans="1:11" ht="14.4" x14ac:dyDescent="0.3">
+      <c r="K4" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="L4" s="4" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="5" spans="1:12" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A5" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="B5" s="3" t="s">
-        <v>61</v>
+      <c r="B5" s="2" t="s">
+        <v>46</v>
       </c>
       <c r="C5" s="3" t="s">
-        <v>23</v>
+        <v>55</v>
       </c>
       <c r="D5" s="3" t="s">
-        <v>43</v>
+        <v>58</v>
       </c>
       <c r="E5" s="3" t="s">
-        <v>44</v>
+        <v>1</v>
       </c>
       <c r="F5" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="G5" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="H5" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="I5" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="J5" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="K5" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="L5" s="4" t="s">
         <v>22</v>
       </c>
-      <c r="G5" s="3" t="s">
-        <v>1</v>
-      </c>
-      <c r="H5" s="3" t="s">
-        <v>1</v>
-      </c>
-      <c r="I5" s="3" t="s">
-        <v>1</v>
-      </c>
-      <c r="J5" s="3" t="s">
-        <v>1</v>
-      </c>
-      <c r="K5" s="4" t="s">
-        <v>49</v>
-      </c>
-    </row>
-    <row r="6" spans="1:11" ht="14.4" x14ac:dyDescent="0.3">
-      <c r="A6" s="3">
-        <v>5</v>
-      </c>
-      <c r="B6" s="3" t="s">
-        <v>61</v>
+    </row>
+    <row r="6" spans="1:12" ht="14.4" x14ac:dyDescent="0.3">
+      <c r="A6" s="3" t="s">
+        <v>68</v>
+      </c>
+      <c r="B6" s="2" t="s">
+        <v>46</v>
       </c>
       <c r="C6" s="3" t="s">
-        <v>25</v>
+        <v>47</v>
       </c>
       <c r="D6" s="3" t="s">
-        <v>26</v>
+        <v>59</v>
       </c>
       <c r="E6" s="3" t="s">
-        <v>27</v>
+        <v>1</v>
       </c>
       <c r="F6" s="3" t="s">
-        <v>28</v>
+        <v>1</v>
       </c>
       <c r="G6" s="3" t="s">
-        <v>55</v>
+        <v>1</v>
       </c>
       <c r="H6" s="3" t="s">
-        <v>56</v>
+        <v>1</v>
       </c>
       <c r="I6" s="3" t="s">
-        <v>22</v>
+        <v>1</v>
       </c>
       <c r="J6" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="K6" s="4" t="s">
+      <c r="K6" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="L6" s="4" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="7" spans="1:11" ht="14.4" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:12" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A7" s="3" t="s">
         <v>13</v>
       </c>
       <c r="B7" s="3" t="s">
-        <v>61</v>
+        <v>54</v>
       </c>
       <c r="C7" s="3" t="s">
-        <v>29</v>
+        <v>60</v>
       </c>
       <c r="D7" s="3" t="s">
-        <v>30</v>
+        <v>1</v>
       </c>
       <c r="E7" s="3" t="s">
-        <v>31</v>
+        <v>1</v>
       </c>
       <c r="F7" s="3" t="s">
-        <v>32</v>
+        <v>1</v>
       </c>
       <c r="G7" s="3" t="s">
-        <v>22</v>
+        <v>1</v>
       </c>
       <c r="H7" s="3" t="s">
         <v>1</v>
@@ -907,117 +974,376 @@
       <c r="J7" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="K7" s="4" t="s">
+      <c r="K7" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="L7" s="4" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="8" spans="1:11" ht="14.4" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:12" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A8" s="3" t="s">
         <v>14</v>
       </c>
       <c r="B8" s="3" t="s">
-        <v>61</v>
+        <v>46</v>
       </c>
       <c r="C8" s="3" t="s">
-        <v>33</v>
+        <v>60</v>
       </c>
       <c r="D8" s="3" t="s">
-        <v>45</v>
+        <v>59</v>
       </c>
       <c r="E8" s="3" t="s">
-        <v>34</v>
+        <v>1</v>
       </c>
       <c r="F8" s="3" t="s">
-        <v>57</v>
+        <v>1</v>
       </c>
       <c r="G8" s="3" t="s">
-        <v>35</v>
+        <v>1</v>
       </c>
       <c r="H8" s="3" t="s">
-        <v>58</v>
+        <v>1</v>
       </c>
       <c r="I8" s="3" t="s">
-        <v>46</v>
+        <v>1</v>
       </c>
       <c r="J8" s="3" t="s">
-        <v>22</v>
-      </c>
-      <c r="K8" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="K8" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="L8" s="4" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="9" spans="1:11" ht="14.4" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:12" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A9" s="3" t="s">
         <v>15</v>
       </c>
-      <c r="B9" s="3" t="s">
+      <c r="B9" s="2" t="s">
+        <v>46</v>
+      </c>
+      <c r="C9" s="3" t="s">
         <v>61</v>
       </c>
-      <c r="C9" s="3" t="s">
-        <v>39</v>
-      </c>
       <c r="D9" s="3" t="s">
-        <v>40</v>
+        <v>62</v>
       </c>
       <c r="E9" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="F9" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="G9" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="H9" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="I9" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="J9" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="K9" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="L9" s="4" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="10" spans="1:12" ht="14.4" x14ac:dyDescent="0.3">
+      <c r="A10" s="3" t="s">
         <v>41</v>
       </c>
-      <c r="F9" s="3" t="s">
+      <c r="B10" s="3" t="s">
+        <v>46</v>
+      </c>
+      <c r="C10" s="3" t="s">
+        <v>63</v>
+      </c>
+      <c r="D10" s="3" t="s">
+        <v>62</v>
+      </c>
+      <c r="E10" s="3" t="s">
+        <v>64</v>
+      </c>
+      <c r="F10" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="G10" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="H10" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="I10" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="J10" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="K10" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="L10" s="4" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="11" spans="1:12" ht="14.4" x14ac:dyDescent="0.3">
+      <c r="A11" s="3" t="s">
+        <v>51</v>
+      </c>
+      <c r="B11" s="3" t="s">
+        <v>46</v>
+      </c>
+      <c r="C11" s="3" t="s">
+        <v>63</v>
+      </c>
+      <c r="D11" s="3" t="s">
+        <v>64</v>
+      </c>
+      <c r="E11" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="F11" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="G11" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="H11" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="I11" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="J11" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="K11" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="L11" s="4" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="12" spans="1:12" ht="14.4" x14ac:dyDescent="0.3">
+      <c r="A12" s="3" t="s">
         <v>42</v>
       </c>
-      <c r="G9" s="3" t="s">
-        <v>59</v>
-      </c>
-      <c r="H9" s="3" t="s">
-        <v>60</v>
-      </c>
-      <c r="I9" s="3" t="s">
-        <v>22</v>
-      </c>
-      <c r="J9" s="3" t="s">
-        <v>1</v>
-      </c>
-      <c r="K9" s="4" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="10" spans="1:11" ht="14.4" x14ac:dyDescent="0.3">
-      <c r="K10" s="6"/>
-    </row>
-    <row r="11" spans="1:11" ht="14.4" x14ac:dyDescent="0.3">
-      <c r="K11" s="6"/>
-    </row>
-    <row r="12" spans="1:11" ht="14.4" x14ac:dyDescent="0.3">
-      <c r="K12" s="6"/>
-    </row>
-    <row r="13" spans="1:11" ht="14.4" x14ac:dyDescent="0.3">
-      <c r="K13" s="6"/>
-    </row>
-    <row r="14" spans="1:11" ht="14.4" x14ac:dyDescent="0.3">
-      <c r="K14" s="6"/>
-    </row>
-    <row r="15" spans="1:11" ht="14.4" x14ac:dyDescent="0.3">
-      <c r="K15" s="6"/>
-    </row>
-    <row r="16" spans="1:11" ht="14.4" x14ac:dyDescent="0.3">
-      <c r="K16" s="5"/>
-    </row>
-    <row r="17" spans="11:11" ht="14.4" x14ac:dyDescent="0.3">
-      <c r="K17" s="5"/>
+      <c r="B12" s="3" t="s">
+        <v>57</v>
+      </c>
+      <c r="C12" s="3" t="s">
+        <v>69</v>
+      </c>
+      <c r="D12" s="3" t="s">
+        <v>70</v>
+      </c>
+      <c r="E12" s="3" t="s">
+        <v>65</v>
+      </c>
+      <c r="F12" s="3" t="s">
+        <v>66</v>
+      </c>
+      <c r="G12" s="3" t="s">
+        <v>67</v>
+      </c>
+      <c r="H12" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="I12" s="8" t="s">
+        <v>1</v>
+      </c>
+      <c r="J12" s="8" t="s">
+        <v>1</v>
+      </c>
+      <c r="K12" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="L12" s="4" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="13" spans="1:12" ht="14.4" x14ac:dyDescent="0.3">
+      <c r="A13" s="3" t="s">
+        <v>43</v>
+      </c>
+      <c r="B13" s="3" t="s">
+        <v>71</v>
+      </c>
+      <c r="C13" s="3" t="s">
+        <v>72</v>
+      </c>
+      <c r="D13" s="3" t="s">
+        <v>67</v>
+      </c>
+      <c r="E13" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="F13" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="G13" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="H13" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="I13" s="8" t="s">
+        <v>1</v>
+      </c>
+      <c r="J13" s="8" t="s">
+        <v>1</v>
+      </c>
+      <c r="K13" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="L13" s="4" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="14" spans="1:12" ht="14.4" x14ac:dyDescent="0.3">
+      <c r="A14" s="3" t="s">
+        <v>44</v>
+      </c>
+      <c r="B14" s="3" t="s">
+        <v>71</v>
+      </c>
+      <c r="C14" s="3" t="s">
+        <v>73</v>
+      </c>
+      <c r="D14" s="3" t="s">
+        <v>67</v>
+      </c>
+      <c r="E14" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="F14" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="G14" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="H14" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="I14" s="8" t="s">
+        <v>1</v>
+      </c>
+      <c r="J14" s="8" t="s">
+        <v>1</v>
+      </c>
+      <c r="K14" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="L14" s="4" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="15" spans="1:12" ht="14.4" x14ac:dyDescent="0.3">
+      <c r="A15" s="3" t="s">
+        <v>45</v>
+      </c>
+      <c r="B15" s="3" t="s">
+        <v>74</v>
+      </c>
+      <c r="C15" s="3" t="s">
+        <v>75</v>
+      </c>
+      <c r="D15" s="3" t="s">
+        <v>76</v>
+      </c>
+      <c r="E15" s="3" t="s">
+        <v>77</v>
+      </c>
+      <c r="F15" s="3" t="s">
+        <v>78</v>
+      </c>
+      <c r="G15" s="3" t="s">
+        <v>79</v>
+      </c>
+      <c r="H15" s="3" t="s">
+        <v>80</v>
+      </c>
+      <c r="I15" s="3" t="s">
+        <v>81</v>
+      </c>
+      <c r="J15" s="3" t="s">
+        <v>83</v>
+      </c>
+      <c r="K15" s="3" t="s">
+        <v>84</v>
+      </c>
+      <c r="L15" s="4" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="16" spans="1:12" ht="14.4" x14ac:dyDescent="0.3">
+      <c r="H16" s="6"/>
+      <c r="L16" s="5"/>
+    </row>
+    <row r="17" spans="8:12" ht="14.4" x14ac:dyDescent="0.3">
+      <c r="H17" s="6"/>
+      <c r="L17" s="5"/>
+    </row>
+    <row r="18" spans="8:12" ht="14.4" x14ac:dyDescent="0.3">
+      <c r="H18" s="6"/>
+    </row>
+    <row r="19" spans="8:12" ht="14.4" x14ac:dyDescent="0.3">
+      <c r="H19" s="6"/>
+    </row>
+    <row r="20" spans="8:12" ht="14.4" x14ac:dyDescent="0.3">
+      <c r="H20" s="6"/>
+    </row>
+    <row r="21" spans="8:12" ht="14.4" x14ac:dyDescent="0.3">
+      <c r="H21" s="7"/>
+    </row>
+    <row r="22" spans="8:12" ht="14.4" x14ac:dyDescent="0.3">
+      <c r="H22" s="6"/>
+    </row>
+    <row r="23" spans="8:12" ht="14.4" x14ac:dyDescent="0.3">
+      <c r="H23" s="6"/>
+    </row>
+    <row r="24" spans="8:12" ht="14.4" x14ac:dyDescent="0.3">
+      <c r="H24" s="6"/>
+    </row>
+    <row r="25" spans="8:12" ht="14.4" x14ac:dyDescent="0.3">
+      <c r="H25" s="6"/>
+    </row>
+    <row r="26" spans="8:12" ht="14.4" x14ac:dyDescent="0.3">
+      <c r="H26" s="6"/>
+    </row>
+    <row r="27" spans="8:12" ht="14.4" x14ac:dyDescent="0.3">
+      <c r="H27" s="6"/>
+    </row>
+    <row r="28" spans="8:12" ht="14.4" x14ac:dyDescent="0.3">
+      <c r="H28" s="6"/>
+    </row>
+    <row r="29" spans="8:12" ht="14.4" x14ac:dyDescent="0.3">
+      <c r="H29" s="6"/>
     </row>
   </sheetData>
+  <phoneticPr fontId="4" type="noConversion"/>
   <hyperlinks>
-    <hyperlink ref="K6" r:id="rId1" xr:uid="{03A8B09A-9C01-4631-98DB-D400E90BD7CA}"/>
-    <hyperlink ref="K7" r:id="rId2" xr:uid="{40A51DF8-DE39-4793-BF3D-6BC4F1993D20}"/>
-    <hyperlink ref="K8" r:id="rId3" xr:uid="{6D5B6790-73EC-4C22-870D-CC2057625F6A}"/>
-    <hyperlink ref="K9" r:id="rId4" xr:uid="{6D111AAD-3B97-4B6A-979C-840900E2B1BC}"/>
-    <hyperlink ref="K2" r:id="rId5" xr:uid="{1F9C7C52-403B-4412-9CBD-13DDE8302F54}"/>
-    <hyperlink ref="K3" r:id="rId6" xr:uid="{4CE25161-A3B3-4F3D-B2E8-1D0556AA61CE}"/>
-    <hyperlink ref="K4" r:id="rId7" xr:uid="{D5510623-90EF-44AA-9E5D-364979C1CC70}"/>
-    <hyperlink ref="K5" r:id="rId8" xr:uid="{1C1B3A3C-72A2-43BC-B17A-E0EC94E1A5A7}"/>
+    <hyperlink ref="L6" r:id="rId1" xr:uid="{03A8B09A-9C01-4631-98DB-D400E90BD7CA}"/>
+    <hyperlink ref="L7" r:id="rId2" xr:uid="{40A51DF8-DE39-4793-BF3D-6BC4F1993D20}"/>
+    <hyperlink ref="L8" r:id="rId3" xr:uid="{6D5B6790-73EC-4C22-870D-CC2057625F6A}"/>
+    <hyperlink ref="L9" r:id="rId4" xr:uid="{6D111AAD-3B97-4B6A-979C-840900E2B1BC}"/>
+    <hyperlink ref="L2" r:id="rId5" xr:uid="{1F9C7C52-403B-4412-9CBD-13DDE8302F54}"/>
+    <hyperlink ref="L4" r:id="rId6" xr:uid="{D5510623-90EF-44AA-9E5D-364979C1CC70}"/>
+    <hyperlink ref="L5" r:id="rId7" xr:uid="{1C1B3A3C-72A2-43BC-B17A-E0EC94E1A5A7}"/>
+    <hyperlink ref="L3" r:id="rId8" xr:uid="{556BAFB9-812E-45D1-BC9F-410D23DAADC2}"/>
+    <hyperlink ref="L10:L15" r:id="rId9" display="\\Resources\\tong hop final wiring\\c7.png" xr:uid="{23C23EDA-FD6A-4B5D-A43F-1551D5D49EA6}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId9"/>
+  <pageSetup orientation="portrait" r:id="rId10"/>
 </worksheet>
 </file>
 
@@ -1026,17 +1352,17 @@
   <dimension ref="A1:G22"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="G12" sqref="G12"/>
+      <selection activeCell="B29" sqref="B29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
-        <v>62</v>
+        <v>25</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>63</v>
+        <v>26</v>
       </c>
       <c r="D1" s="1"/>
       <c r="E1" s="1"/>
@@ -1045,10 +1371,10 @@
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A2" s="1" t="s">
-        <v>64</v>
+        <v>27</v>
       </c>
       <c r="C2" s="3" t="s">
-        <v>65</v>
+        <v>28</v>
       </c>
       <c r="D2" s="1"/>
       <c r="E2" s="1"/>
@@ -1057,10 +1383,10 @@
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A3" s="1" t="s">
-        <v>66</v>
+        <v>29</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>67</v>
+        <v>30</v>
       </c>
       <c r="D3" s="1"/>
       <c r="E3" s="1"/>
@@ -1069,10 +1395,10 @@
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A4" s="1" t="s">
-        <v>68</v>
+        <v>31</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>69</v>
+        <v>32</v>
       </c>
       <c r="D4" s="1"/>
       <c r="E4" s="1"/>
@@ -1081,10 +1407,10 @@
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A5" s="1" t="s">
-        <v>70</v>
+        <v>33</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>71</v>
+        <v>34</v>
       </c>
       <c r="D5" s="1"/>
       <c r="E5" s="1"/>
@@ -1093,10 +1419,10 @@
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A6" s="1" t="s">
-        <v>72</v>
+        <v>35</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>73</v>
+        <v>36</v>
       </c>
       <c r="D6" s="1"/>
       <c r="E6" s="1"/>
@@ -1105,10 +1431,10 @@
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A7" s="1" t="s">
-        <v>74</v>
+        <v>37</v>
       </c>
       <c r="C7" s="1" t="s">
-        <v>75</v>
+        <v>38</v>
       </c>
       <c r="D7" s="1"/>
       <c r="E7" s="1"/>
@@ -1117,10 +1443,10 @@
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A8" s="1" t="s">
-        <v>76</v>
+        <v>39</v>
       </c>
       <c r="C8" s="1" t="s">
-        <v>77</v>
+        <v>40</v>
       </c>
       <c r="D8" s="1"/>
       <c r="E8" s="1"/>
@@ -1165,66 +1491,66 @@
     </row>
     <row r="15" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A15" s="1" t="s">
-        <v>62</v>
+        <v>25</v>
       </c>
       <c r="B15" s="1" t="s">
-        <v>63</v>
+        <v>26</v>
       </c>
     </row>
     <row r="16" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A16" s="1" t="s">
-        <v>64</v>
+        <v>27</v>
       </c>
       <c r="B16" s="3" t="s">
-        <v>65</v>
+        <v>28</v>
       </c>
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A17" s="1" t="s">
-        <v>66</v>
+        <v>29</v>
       </c>
       <c r="B17" s="1" t="s">
-        <v>67</v>
+        <v>30</v>
       </c>
     </row>
     <row r="18" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A18" s="1" t="s">
-        <v>68</v>
+        <v>31</v>
       </c>
       <c r="B18" s="1" t="s">
-        <v>69</v>
+        <v>32</v>
       </c>
     </row>
     <row r="19" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A19" s="1" t="s">
-        <v>70</v>
+        <v>33</v>
       </c>
       <c r="B19" s="1" t="s">
-        <v>71</v>
+        <v>34</v>
       </c>
     </row>
     <row r="20" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A20" s="1" t="s">
-        <v>72</v>
+        <v>35</v>
       </c>
       <c r="B20" s="1" t="s">
-        <v>73</v>
+        <v>36</v>
       </c>
     </row>
     <row r="21" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A21" s="1" t="s">
-        <v>74</v>
+        <v>37</v>
       </c>
       <c r="B21" s="1" t="s">
-        <v>75</v>
+        <v>38</v>
       </c>
     </row>
     <row r="22" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A22" s="1" t="s">
-        <v>76</v>
+        <v>39</v>
       </c>
       <c r="B22" s="1" t="s">
-        <v>77</v>
+        <v>40</v>
       </c>
     </row>
   </sheetData>

</xml_diff>